<commit_message>
LLF_sym now properly takes hazard function as parameter
</commit_message>
<xml_diff>
--- a/covariate_data.xlsx
+++ b/covariate_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\repos\Covariate_Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aubertine/Documents/repos/Covariate_Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{043782AC-B692-4F48-A657-E5BC4320952B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F3B09A-22F9-C248-B481-80773C829260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="1356" windowWidth="17436" windowHeight="12204" activeTab="1" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
+    <workbookView xWindow="2500" yWindow="1360" windowWidth="17440" windowHeight="12200" activeTab="1" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
   </bookViews>
   <sheets>
     <sheet name="DS1" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>kVec</t>
   </si>
@@ -43,13 +40,13 @@
     <t>cVec</t>
   </si>
   <si>
-    <t>Evec</t>
+    <t>T</t>
   </si>
   <si>
-    <t>FVec</t>
+    <t>eVec</t>
   </si>
   <si>
-    <t>Fvec</t>
+    <t>fVec</t>
   </si>
 </sst>
 </file>
@@ -404,20 +401,20 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -426,7 +423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -443,7 +440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -460,7 +457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -477,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -494,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -511,7 +508,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -528,7 +525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -545,7 +542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -562,7 +559,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -579,7 +576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -596,7 +593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -613,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -630,7 +627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -647,7 +644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -664,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -681,7 +678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -698,7 +695,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -725,29 +722,29 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -764,7 +761,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -781,7 +778,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -798,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -815,7 +812,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -832,7 +829,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -849,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -866,7 +863,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -883,7 +880,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -900,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -917,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -934,7 +931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -951,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -968,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Tab 1 shows all combinations of metrics
New combinations don't run yet.
</commit_message>
<xml_diff>
--- a/covariate_data.xlsx
+++ b/covariate_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aubertine/Documents/repos/Covariate_Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F3B09A-22F9-C248-B481-80773C829260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59085AC-39B6-CA46-9D2D-43CB839F510A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="1360" windowWidth="17440" windowHeight="12200" activeTab="1" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
   </bookViews>
@@ -722,7 +722,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Input data read based on column headers
Also added list of models and metric combinations that didn't converge on tab 2
</commit_message>
<xml_diff>
--- a/covariate_data.xlsx
+++ b/covariate_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aubertine/Documents/repos/Covariate_Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59085AC-39B6-CA46-9D2D-43CB839F510A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E821EA7-0EB1-D146-80DF-E2483DBE2EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1360" windowWidth="17440" windowHeight="12200" activeTab="1" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
+    <workbookView xWindow="2500" yWindow="1360" windowWidth="17440" windowHeight="12200" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
   </bookViews>
   <sheets>
     <sheet name="DS1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
-    <t>kVec</t>
-  </si>
-  <si>
     <t>cVec</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>fVec</t>
+  </si>
+  <si>
+    <t>FC</t>
   </si>
 </sst>
 </file>
@@ -400,27 +400,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA58DA2-4B17-49DD-A384-32C5A179A21B}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -721,27 +721,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3724057A-E4DA-4229-B436-3ADE45F36CF0}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Intensity view is now a bar chart
</commit_message>
<xml_diff>
--- a/covariate_data.xlsx
+++ b/covariate_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aubertine/Documents/repos/Covariate_Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\repos\Covariate_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E821EA7-0EB1-D146-80DF-E2483DBE2EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE9F2A5-8466-46C6-A1CF-07DFFDB405AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1360" windowWidth="17440" windowHeight="12200" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E306A3B3-E968-484E-9853-F350328284C5}"/>
   </bookViews>
   <sheets>
     <sheet name="DS1" sheetId="1" r:id="rId1"/>
@@ -400,13 +400,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA58DA2-4B17-49DD-A384-32C5A179A21B}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -423,7 +423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -440,7 +440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -457,7 +457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -508,7 +508,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -525,7 +525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -542,7 +542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -559,7 +559,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -576,7 +576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -593,7 +593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -627,7 +627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -644,7 +644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -661,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -678,7 +678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -695,7 +695,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -725,9 +725,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -761,7 +761,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -778,7 +778,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -795,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -812,7 +812,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -829,7 +829,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -846,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -863,7 +863,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -880,7 +880,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -897,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -914,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -931,7 +931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -948,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -965,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>